<commit_message>
Indkøb reserve dele bms fortsat
</commit_message>
<xml_diff>
--- a/Documents/Shopping/Komponenter til rådighed BMS.xlsx
+++ b/Documents/Shopping/Komponenter til rådighed BMS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jens Peter Nymann\Documents\GitHub\PRJ4\Documents\Shopping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Studie-PC\Documents\GitHub\PRJ4\Documents\Shopping\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="127">
   <si>
     <t>Antal</t>
   </si>
@@ -56,12 +56,6 @@
     <t>BAV19W</t>
   </si>
   <si>
-    <t>bq76PL536AQ1</t>
-  </si>
-  <si>
-    <t>Not good</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/panasonic-electronic-components/erja1aj270u/resistor-wide-term-27r-1-33w-5/dp/1670314</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>Etc</t>
   </si>
   <si>
-    <t>http://www.ti.com/lit/ds/symlink/sn74aup1g14.pdf</t>
-  </si>
-  <si>
     <t>http://www.mouser.dk/ProductDetail/Panasonic/DB2232000L/?qs=5MvhVKkHFQWgfo8hpbrqtA%3d%3d</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>http://dk.farnell.com/multicomp/mc0603b104j160ct/cap-mlcc-x7r-100nf-16v-0603/dp/2320813</t>
   </si>
   <si>
-    <t>0,1 uF</t>
-  </si>
-  <si>
     <t>MC0603B103J500CT</t>
   </si>
   <si>
@@ -347,21 +335,12 @@
     <t>NTC Resi</t>
   </si>
   <si>
-    <t>10000 Ohm</t>
-  </si>
-  <si>
-    <t>http://dk.farnell.com/panasonic-electronic-components/ertj1vg103fa/thermistor-ntc-0603-10k/dp/1892611/false</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/texas-instruments/bq76pl536atpaptq1/batt-prot-li-ion-27v-htqfp-64/dp/2492116?CMP=GRHB-FINDCHIPS</t>
   </si>
   <si>
     <t>MH 5</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/texas-instruments/opa333aidg4/op-amp-350khz-0-16v-us-2uv-soic/dp/1230458/false</t>
-  </si>
-  <si>
     <t>OPA333AIDG4</t>
   </si>
   <si>
@@ -372,6 +351,60 @@
   </si>
   <si>
     <t>LT6656B-2.5</t>
+  </si>
+  <si>
+    <t>AVR CAN (AT90CAN128)</t>
+  </si>
+  <si>
+    <t>RELÆ</t>
+  </si>
+  <si>
+    <t>BQ76PL536ATPAPTQ1</t>
+  </si>
+  <si>
+    <t>MH 8</t>
+  </si>
+  <si>
+    <t>10000 Ohm MH 5</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/olimex/avr-can/at90can128-can-rs232-dev-board/dp/1776310?selectedCategoryId=&amp;exaMfpn=true&amp;categoryId=&amp;searchRef=SearchLookAhead&amp;iscrfnonsku=false</t>
+  </si>
+  <si>
+    <t>MH 1</t>
+  </si>
+  <si>
+    <t>74HCT04D</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/nxp/74hct04d/74hct-cmos-smd-74hct04-soic14/dp/1085299/false</t>
+  </si>
+  <si>
+    <t>27 Ohm MH 15</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/texas-instruments/sn74aup1g14dbvt/logic-inverter-sch-trig-sgl-5sot23/dp/1741194?selectedCategoryId=&amp;exaMfpn=true&amp;categoryId=&amp;searchRef=SearchLookAhead&amp;iscrfnonsku=false</t>
+  </si>
+  <si>
+    <t>0,1 uF MH20</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/bourns/cr0603-fx-1002elf/res-thick-film-10k-1-0-1w-0603/dp/2008341/false</t>
+  </si>
+  <si>
+    <t>10000 Ohm MH 20</t>
+  </si>
+  <si>
+    <t>CR0603-FX-1002ELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230k, 960k 40k Ohm kan ikke findes på farnell </t>
+  </si>
+  <si>
+    <t>ER IKKE PÅ PRINTET TIL BMS</t>
+  </si>
+  <si>
+    <t>MH 5 Set på printet</t>
   </si>
 </sst>
 </file>
@@ -471,6 +504,7 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,11 +517,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Kontrollér celle" xfId="1" builtinId="23"/>
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -512,8 +545,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:E50" totalsRowShown="0" tableBorderDxfId="0">
-  <autoFilter ref="A4:E50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:E56" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="A4:E56"/>
   <sortState ref="A5:E15">
     <sortCondition ref="A4:A15"/>
   </sortState>
@@ -529,9 +562,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -569,7 +602,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -641,7 +674,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -791,38 +824,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X49"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -833,14 +866,14 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -851,7 +884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -862,10 +895,10 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -875,11 +908,14 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -890,9 +926,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -901,363 +937,363 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>26</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>30</v>
       </c>
       <c r="B14">
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>34</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>36</v>
       </c>
       <c r="B16">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>45</v>
       </c>
       <c r="B19">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>47</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>48</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>51</v>
       </c>
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>49</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>52</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>53</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>56</v>
       </c>
       <c r="B23">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>58</v>
       </c>
       <c r="B24">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>65</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>69</v>
       </c>
       <c r="B27">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>68</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>72</v>
       </c>
       <c r="B28">
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B29">
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>79</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1265,16 +1301,19 @@
       <c r="C31" t="s">
         <v>7</v>
       </c>
+      <c r="D31" t="s">
+        <v>125</v>
+      </c>
       <c r="E31" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="X31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B32">
         <v>22</v>
@@ -1283,43 +1322,43 @@
         <v>6</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B33">
         <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>86</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -1328,70 +1367,60 @@
         <v>6</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B37">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>103</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1399,53 +1428,121 @@
       <c r="C41" t="s">
         <v>4</v>
       </c>
+      <c r="D41" t="s">
+        <v>104</v>
+      </c>
       <c r="E41" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
+        <v>104</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>110</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" t="s">
+        <v>122</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D49" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>126</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1455,43 +1552,46 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E10" r:id="rId1"/>
-    <hyperlink ref="E7" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E11" r:id="rId4"/>
-    <hyperlink ref="E12" r:id="rId5"/>
-    <hyperlink ref="E13" r:id="rId6"/>
-    <hyperlink ref="E14" r:id="rId7"/>
-    <hyperlink ref="E16" r:id="rId8"/>
-    <hyperlink ref="E17" r:id="rId9"/>
-    <hyperlink ref="E19" r:id="rId10"/>
-    <hyperlink ref="E18" r:id="rId11"/>
-    <hyperlink ref="E20" r:id="rId12"/>
-    <hyperlink ref="E21" r:id="rId13"/>
-    <hyperlink ref="E22" r:id="rId14"/>
-    <hyperlink ref="E23" r:id="rId15"/>
-    <hyperlink ref="E24" r:id="rId16"/>
-    <hyperlink ref="E25" r:id="rId17"/>
-    <hyperlink ref="E26" r:id="rId18"/>
-    <hyperlink ref="E27" r:id="rId19"/>
-    <hyperlink ref="E28" r:id="rId20"/>
-    <hyperlink ref="E29" r:id="rId21"/>
-    <hyperlink ref="E30" r:id="rId22"/>
-    <hyperlink ref="E31" r:id="rId23"/>
-    <hyperlink ref="E32" r:id="rId24"/>
-    <hyperlink ref="E33" r:id="rId25"/>
-    <hyperlink ref="E34" r:id="rId26"/>
-    <hyperlink ref="E35" r:id="rId27"/>
-    <hyperlink ref="E36" r:id="rId28"/>
-    <hyperlink ref="E38" r:id="rId29"/>
-    <hyperlink ref="E41" r:id="rId30"/>
-    <hyperlink ref="E42" r:id="rId31"/>
-    <hyperlink ref="E43" r:id="rId32"/>
-    <hyperlink ref="E49" r:id="rId33"/>
+    <hyperlink ref="E6" r:id="rId2"/>
+    <hyperlink ref="E11" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId4"/>
+    <hyperlink ref="E13" r:id="rId5"/>
+    <hyperlink ref="E14" r:id="rId6"/>
+    <hyperlink ref="E16" r:id="rId7"/>
+    <hyperlink ref="E17" r:id="rId8"/>
+    <hyperlink ref="E19" r:id="rId9"/>
+    <hyperlink ref="E18" r:id="rId10"/>
+    <hyperlink ref="E20" r:id="rId11"/>
+    <hyperlink ref="E21" r:id="rId12"/>
+    <hyperlink ref="E22" r:id="rId13"/>
+    <hyperlink ref="E23" r:id="rId14"/>
+    <hyperlink ref="E24" r:id="rId15"/>
+    <hyperlink ref="E25" r:id="rId16"/>
+    <hyperlink ref="E26" r:id="rId17"/>
+    <hyperlink ref="E27" r:id="rId18"/>
+    <hyperlink ref="E28" r:id="rId19"/>
+    <hyperlink ref="E29" r:id="rId20"/>
+    <hyperlink ref="E30" r:id="rId21"/>
+    <hyperlink ref="E31" r:id="rId22"/>
+    <hyperlink ref="E32" r:id="rId23"/>
+    <hyperlink ref="E33" r:id="rId24"/>
+    <hyperlink ref="E34" r:id="rId25"/>
+    <hyperlink ref="E35" r:id="rId26"/>
+    <hyperlink ref="E36" r:id="rId27"/>
+    <hyperlink ref="E38" r:id="rId28"/>
+    <hyperlink ref="E41" r:id="rId29"/>
+    <hyperlink ref="E49" r:id="rId30"/>
+    <hyperlink ref="E9" r:id="rId31"/>
+    <hyperlink ref="E45" r:id="rId32"/>
+    <hyperlink ref="E51" r:id="rId33"/>
+    <hyperlink ref="E7" r:id="rId34"/>
+    <hyperlink ref="E48" r:id="rId35"/>
+    <hyperlink ref="E42:E43" r:id="rId36" display="http://dk.farnell.com/fairchild-semiconductor/hcpl2731sd/optocoupler-darlington-2-5kv-smdip/dp/2453182/false"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
   <tableParts count="1">
-    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId38"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>